<commit_message>
Change terminal storage amounts to input parameters
Move terminal storage amounts (days) for compressed and liquid hydrogen to dictionary of input parameters for the "calcs" function. Update "input_params" Excel file.
</commit_message>
<xml_diff>
--- a/systems2atoms/systems/inputs/input_params_baseline.xlsx
+++ b/systems2atoms/systems/inputs/input_params_baseline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/GitHub/systems2atoms/systems2atoms/systems/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{401E820F-D25F-3D46-84BE-224BE0C8BBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{401E820F-D25F-3D46-84BE-224BE0C8BBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A63418F1-8263-41C5-8F45-0553FE2407F8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,7 +406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT1" authorId="0" shapeId="0" xr:uid="{6CEB0D03-8142-4461-B5D8-E2E1F9D69928}">
+    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{6CEB0D03-8142-4461-B5D8-E2E1F9D69928}">
       <text>
         <r>
           <rPr>
@@ -430,7 +430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU1" authorId="0" shapeId="0" xr:uid="{A7F3BD7A-BC91-4F82-8B30-22EC15A227B3}">
+    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{A7F3BD7A-BC91-4F82-8B30-22EC15A227B3}">
       <text>
         <r>
           <rPr>
@@ -685,7 +685,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>run #</t>
   </si>
@@ -850,6 +850,12 @@
   </si>
   <si>
     <t>hydr. electrolyzer cell area (m^2/cell)</t>
+  </si>
+  <si>
+    <t>terminal compressed hydrogen storage amount (days)</t>
+  </si>
+  <si>
+    <t>terminal liquid hydrogen storage amount (days)</t>
   </si>
 </sst>
 </file>
@@ -1739,13 +1745,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV5"/>
+  <dimension ref="A1:AX5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AI3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AM1" sqref="AM1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1787,20 +1793,22 @@
     <col min="35" max="35" width="31" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="31" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="29" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="50" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="31" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="29" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="43" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="43" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -1913,40 +1921,46 @@
         <v>45</v>
       </c>
       <c r="AL1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -2039,7 +2053,7 @@
         <v>0</v>
       </c>
       <c r="AE2" s="1">
-        <f t="shared" ref="AE2:AE5" si="1">D2/2.016/S2*Q2/AN2/24/3600*F2</f>
+        <f t="shared" ref="AE2:AE5" si="1">D2/2.016/S2*Q2/AP2/24/3600*F2</f>
         <v>2.6426092969379242</v>
       </c>
       <c r="AF2" s="1">
@@ -2062,40 +2076,46 @@
         <v>0.25</v>
       </c>
       <c r="AL2" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1">
         <v>300</v>
       </c>
-      <c r="AM2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="1">
+      <c r="AO2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="1">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AO2" s="1">
+      <c r="AQ2" s="1">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AP2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="1">
+      <c r="AR2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="1">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AR2" s="1">
+      <c r="AT2" s="1">
         <v>3500</v>
       </c>
-      <c r="AS2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AT2" s="1">
-        <v>0</v>
-      </c>
       <c r="AU2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -2212,40 +2232,46 @@
         <v>0.25</v>
       </c>
       <c r="AL3">
+        <v>0.25</v>
+      </c>
+      <c r="AM3">
+        <v>1</v>
+      </c>
+      <c r="AN3">
         <v>300</v>
       </c>
-      <c r="AM3">
-        <v>1</v>
-      </c>
-      <c r="AN3">
+      <c r="AO3">
+        <v>1</v>
+      </c>
+      <c r="AP3">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AO3">
+      <c r="AQ3">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AP3">
-        <v>1</v>
-      </c>
-      <c r="AQ3">
+      <c r="AR3">
+        <v>1</v>
+      </c>
+      <c r="AS3">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AR3">
+      <c r="AT3">
         <v>3500</v>
       </c>
-      <c r="AS3">
-        <v>1</v>
-      </c>
-      <c r="AT3">
-        <v>0</v>
-      </c>
       <c r="AU3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2362,40 +2388,46 @@
         <v>0.25</v>
       </c>
       <c r="AL4">
+        <v>0.25</v>
+      </c>
+      <c r="AM4">
+        <v>1</v>
+      </c>
+      <c r="AN4">
         <v>300</v>
       </c>
-      <c r="AM4">
-        <v>1</v>
-      </c>
-      <c r="AN4">
+      <c r="AO4">
+        <v>1</v>
+      </c>
+      <c r="AP4">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AO4">
+      <c r="AQ4">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AP4">
-        <v>1</v>
-      </c>
-      <c r="AQ4">
+      <c r="AR4">
+        <v>1</v>
+      </c>
+      <c r="AS4">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AR4">
+      <c r="AT4">
         <v>3500</v>
       </c>
-      <c r="AS4">
-        <v>1</v>
-      </c>
-      <c r="AT4">
-        <v>0</v>
-      </c>
       <c r="AU4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>0</v>
+      </c>
+      <c r="AX4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -2512,41 +2544,47 @@
         <v>0.25</v>
       </c>
       <c r="AL5">
+        <v>0.25</v>
+      </c>
+      <c r="AM5">
+        <v>1</v>
+      </c>
+      <c r="AN5">
         <v>300</v>
       </c>
-      <c r="AM5">
-        <v>1</v>
-      </c>
-      <c r="AN5">
+      <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AO5">
+      <c r="AQ5">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AP5">
-        <v>1</v>
-      </c>
-      <c r="AQ5">
+      <c r="AR5">
+        <v>1</v>
+      </c>
+      <c r="AS5">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AR5">
+      <c r="AT5">
         <v>3500</v>
       </c>
-      <c r="AS5">
-        <v>1</v>
-      </c>
-      <c r="AT5">
-        <v>0</v>
-      </c>
       <c r="AU5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
+      </c>
+      <c r="AX5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:AV5">
+  <conditionalFormatting sqref="C3:AX5">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>C3&lt;&gt;C$2</formula>
     </cfRule>
@@ -2791,15 +2829,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="72d00a49-d4df-4ae2-8448-0e7c38748169">
@@ -2808,6 +2837,15 @@
     <TaxCatchAll xmlns="cdbd341c-9425-4527-8200-dbc5093c0c26" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2831,14 +2869,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB52D826-44CA-4104-AA1D-CE7759CCAD0E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA3A8468-9818-4804-84E1-135F70628E6B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2847,4 +2877,12 @@
     <ds:schemaRef ds:uri="cdbd341c-9425-4527-8200-dbc5093c0c26"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB52D826-44CA-4104-AA1D-CE7759CCAD0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix electrolyzer fixed costs and energy
Use terminal LOHC mass flowrate (instead of molar flowrate) as the target flowrate for scaling LOHC electrolyzer area and energy. Fix both code and input Excel file. (Note: Previously mixed up molar and mass flowrates. Formic acid results were not impacted because of a similar mismatch in input Excel file.)
</commit_message>
<xml_diff>
--- a/systems2atoms/systems/inputs/input_params_baseline.xlsx
+++ b/systems2atoms/systems/inputs/input_params_baseline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/GitHub/systems2atoms/systems2atoms/systems/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{401E820F-D25F-3D46-84BE-224BE0C8BBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A63418F1-8263-41C5-8F45-0553FE2407F8}"/>
+  <xr:revisionPtr revIDLastSave="706" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDA50D74-30F0-4FAB-9A30-D15EFF0A634E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -38,7 +41,7 @@
     <author>Yuan, Mengyao</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{E69AF14B-AA4E-4E26-959E-FBBD27782D10}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{F534F6D7-4901-4F6A-8CC7-2E2C2D99DD41}">
       <text>
         <r>
           <rPr>
@@ -46,7 +49,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -55,14 +58,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Identifier; passthrough input (not used in calculations).</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{CD81A55F-A99E-4A56-B972-678F29DCB64C}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{149A9FCB-A214-484B-ACFA-43A1F3D93045}">
       <text>
         <r>
           <rPr>
@@ -70,7 +73,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -79,14 +82,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Used for output file #. Need to be different for each run.</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{13073E9C-D811-47E4-B2BE-7D12539399FD}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{07439F81-7639-4D31-9818-6B9E6FB8B6C2}">
       <text>
         <r>
           <rPr>
@@ -94,7 +97,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -103,14 +106,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Dollar year of calculated costs.</t>
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{ACA71E89-892C-48A7-882C-1D446A4F3744}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{915D608B-C9BE-457D-BD52-CFBE5A52D97D}">
       <text>
         <r>
           <rPr>
@@ -118,7 +121,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -127,14 +130,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Use in delivery pathway name (in output files).</t>
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{E91F5129-45DF-4C7E-98CB-9EB0ECA2B407}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{C7611B61-73DE-427C-A544-5D1F8E91B3BD}">
       <text>
         <r>
           <rPr>
@@ -142,7 +145,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -151,14 +154,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 At target transport and storage conditions for given LOHC.</t>
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{1FA48B68-1334-4FAC-BF0B-33E0BBEB747F}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{5164F6DD-2EED-4C08-96E3-F9BB8501BC6D}">
       <text>
         <r>
           <rPr>
@@ -178,12 +181,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Accepted values are "thermo", "electro", or "purchase".
-Currently "thermo" formic acid production calculations are incomplete.</t>
+Used for mass balance. If feed is not H2 (e.g., H2O), convert to stoichiometric coefficent for H2.</t>
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{BE111B58-CF02-47A8-A900-0FE1C58D67F9}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{7B439CF8-FCC0-4775-90A9-4F164A871452}">
       <text>
         <r>
           <rPr>
@@ -203,29 +205,187 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Currently not used.
-Intended for "thermo" formic acid production calculations, which are currently incomplete.</t>
+Used for calculating CO2 recycling costs and dehydrogenation byproduct emissions. If CO2 is not used or produced in the reactions, fill out 0.</t>
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{6762C2A9-ED90-4F8A-ACBA-004F9BE735F8}">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{3BA61561-4F80-4528-AEF8-1B98AE0EDD46}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Accepted values are "thermo", "electro", or "purchase".
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Currently "thermo" formic acid production calculations are incomplete.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{CE96F9E7-E862-4E63-9E2A-7C2E1947B8B3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yuan, Mengyao:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Currently not used.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Intended for "thermo" formic acid production calculations, which are currently incomplete.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{138103C3-8219-4014-8B1C-89126F5B990C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yuan, Mengyao:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Placeholder.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Used for "thermo" formic acid production calculations, which are currently incomplete.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{164166BC-1CC9-4991-B115-786C2E89C324}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yuan, Mengyao:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Placeholder.
@@ -233,7 +393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{D04DD905-76F8-48FD-B1A3-7586587FD9C8}">
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{D0E08A76-FEDD-465B-B1F6-7EB1A4DE89A4}">
       <text>
         <r>
           <rPr>
@@ -241,7 +401,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -250,7 +410,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Placeholder.
@@ -258,7 +418,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{B12FB536-677E-448D-90D6-6B05614E32BF}">
+    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{3C10C9CD-EDDD-4D19-804C-ADAEB111B7E9}">
       <text>
         <r>
           <rPr>
@@ -266,7 +426,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -275,7 +435,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Placeholder.
@@ -283,7 +443,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{85A575E1-5A04-4DA1-BB58-B3BCF3F55057}">
+    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{D4E417D2-A260-4ADD-92C4-7C5768A1F3F3}">
       <text>
         <r>
           <rPr>
@@ -291,7 +451,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -300,7 +460,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Placeholder.
@@ -308,7 +468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{53065B57-609C-4573-9453-189D2C9F884E}">
+    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{3AA9C85D-21E4-4C29-91E6-8D37525B5FC5}">
       <text>
         <r>
           <rPr>
@@ -316,7 +476,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -325,7 +485,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Placeholder.
@@ -333,7 +493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{0F29EAB0-39C2-4C84-B012-71138AA8BEA4}">
+    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{8B76EE6B-3B7E-457B-8FE3-545745C9ECC6}">
       <text>
         <r>
           <rPr>
@@ -341,7 +501,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -350,15 +510,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Placeholder.
-Used for "thermo" formic acid production calculations, which are currently incomplete.</t>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Currently not used.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{481A628E-2100-4163-B507-26D09F915FE1}">
+    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{30D85B9E-15E4-4604-8CAA-32B765517170}">
       <text>
         <r>
           <rPr>
@@ -366,7 +525,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -375,14 +534,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Currently not used.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{7B3A9B9D-8EFE-4593-9AE8-1DC567406CA3}">
+    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{3CEB65E5-8338-4451-AB5C-EBCA3C4962CC}">
       <text>
         <r>
           <rPr>
@@ -390,7 +549,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -399,14 +558,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Currently not used.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{6CEB0D03-8142-4461-B5D8-E2E1F9D69928}">
+    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{405935AC-9727-4D69-942C-356191EE2051}">
       <text>
         <r>
           <rPr>
@@ -414,7 +573,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -423,14 +582,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Currently not used.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{A7F3BD7A-BC91-4F82-8B30-22EC15A227B3}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{51C2103A-A013-48C5-9D57-2E5D4E766D9C}">
       <text>
         <r>
           <rPr>
@@ -438,7 +597,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -447,14 +606,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Currently not used.</t>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Example baseline inputs.</t>
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{1E7F2DFD-E28F-40BA-BF84-2656FEB4603F}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{9119AC3A-05FD-4B3D-A32F-E6D463BD3ACA}">
       <text>
         <r>
           <rPr>
@@ -462,23 +621,24 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Yuan, Mengyao:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Example baseline inputs.</t>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Yuan, Mengyao:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Annual average retail electricity price for California industrial sector in 2022.
+Reference: U.S. Energy Information Administration, Electric Power Annual 2022, Washington, DC, 2023.</t>
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{214B6BAD-4E8B-4B8C-9A1B-A05799FF452B}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{6580F6B2-EE3A-48CB-B777-1841E43A5BCE}">
       <text>
         <r>
           <rPr>
@@ -486,24 +646,24 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Yuan, Mengyao:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Annual average retail electricity price for California industrial sector in 2022.
-Reference: U.S. Energy Information Administration, Electric Power Annual 2022, Washington, DC, 2023.</t>
+            <family val="2"/>
+          </rPr>
+          <t>Yuan, Mengyao:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Annual average diesel price (on-highway, all types) in California in 2022.
+Reference: U.S. Energy Information Administration, Weekly Retail Gasoline and Diesel Prices. https://www.eia.gov/dnav/pet/pet_pri_gnd_dcus_nus_a.htm.</t>
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{CD78496C-361F-4AA2-A7B5-C49F252EFCEA}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{45965082-B84E-4012-B1F3-2B95F4D1F942}">
       <text>
         <r>
           <rPr>
@@ -511,7 +671,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -520,15 +680,15 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Annual average diesel price (on-highway, all types) in California in 2022.
-Reference: U.S. Energy Information Administration, Weekly Retail Gasoline and Diesel Prices. https://www.eia.gov/dnav/pet/pet_pri_gnd_dcus_nus_a.htm.</t>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+2021 State Electricity Profiles, California, CO2 emissions rate. Converted from lb/MWh.
+https://www.eia.gov/electricity/state/california/</t>
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{6E182C7D-C4A7-4883-AEF9-502B2BDB4F6F}">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{7CAF2FE8-6AE9-451E-AA78-4E49C5EC0056}">
       <text>
         <r>
           <rPr>
@@ -536,7 +696,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -545,15 +705,15 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-2021 State Electricity Profiles, California, CO2 emissions rate. Converted from lb/MWh.
-https://www.eia.gov/electricity/state/california/</t>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+EPA, "Greenhouse Gases Equivalencies Calculator - Calculations and References", "Gallons of diesel consumed".
+https://www.epa.gov/energy/greenhouse-gases-equivalencies-calculator-calculations-and-references</t>
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{A4A58B15-9A8C-4A09-8F6B-3EA07859A592}">
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{78230218-071F-43FB-99E0-1C55D385CD29}">
       <text>
         <r>
           <rPr>
@@ -561,7 +721,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -570,40 +730,108 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-EPA, "Greenhouse Gases Equivalencies Calculator - Calculations and References", "Gallons of diesel consumed".
-https://www.epa.gov/energy/greenhouse-gases-equivalencies-calculator-calculations-and-references</t>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Levelized cost of fuel production for hydrogen produced from electrolysis with Inflation Reduction Act tax credits.
+Cheng et al., 2023, Environ. Sci. Technol. https://doi.org/10.1021/acs.est.3c03063.</t>
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{ED41E46E-89DA-4353-BA76-6AC3E7C714C9}">
+    <comment ref="AG2" authorId="0" shapeId="0" xr:uid="{8205285B-115C-47F0-8185-1199E3B70079}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Levelized cost of fuel production for hydrogen produced from electrolysis with Inflation Reduction Act tax credits.
-Cheng et al., 2023, Environ. Sci. Technol. https://doi.org/10.1021/acs.est.3c03063.</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Cell voltage for hydrogen oxidation. Calculated assuming a cell voltage of 2.5 V for water oxidation [1,2] and a reversible potential for water oxidation relative to hydrogen oxidation of 1.23 V (i.e., 2.5 V − 1.23 V = 1.27 V) [3].
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[1] B. S. Crandall, T. Brix, R. S. Weber and F. Jiao, Energ Fuel, 2022, 37, 1441-1450.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[2] M. Ramdin, A. R. T. Morrison, M. de Groen, R. van Haperen, R. de Kler, L. J. P. van den Broeke, J. P. M. Trusler, W. de Jong and T. J. H. Vlugt, Ind Eng Chem Res, 2019, 58, 1834-1847.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[3] W. Q. Li, J. T. Feaster, S. A. Akhade, J. T. Davis, A. A. Wong, V. A. Beck, J. B. Varley, S. A. Hawks, M. Stadermann, C. Hahn, R. D. Aines, E. B. Duoss and S. E. Baker, ACS Sustain Chem Eng, 2021, 9, 14678-14689.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AG2" authorId="0" shapeId="0" xr:uid="{C26BA404-EDC2-4E3C-8D61-9D1F07B5884C}">
+    <comment ref="AH2" authorId="0" shapeId="0" xr:uid="{620FA4F2-8917-46B3-ABA1-BF61E4D757BE}">
       <text>
         <r>
           <rPr>
@@ -611,7 +839,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -620,17 +848,15 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Cell voltage for hydrogen oxidation. Calculated assuming a cell voltage of 2.5 V for water oxidation [1,2] and a reversible potential for water oxidation relative to hydrogen oxidation of 1.23 V (i.e., 2.5 V − 1.23 V = 1.27 V) [3].
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 [1] B. S. Crandall, T. Brix, R. S. Weber and F. Jiao, Energ Fuel, 2022, 37, 1441-1450.
-[2] M. Ramdin, A. R. T. Morrison, M. de Groen, R. van Haperen, R. de Kler, L. J. P. van den Broeke, J. P. M. Trusler, W. de Jong and T. J. H. Vlugt, Ind Eng Chem Res, 2019, 58, 1834-1847.
-[3] W. Q. Li, J. T. Feaster, S. A. Akhade, J. T. Davis, A. A. Wong, V. A. Beck, J. B. Varley, S. A. Hawks, M. Stadermann, C. Hahn, R. D. Aines, E. B. Duoss and S. E. Baker, ACS Sustain Chem Eng, 2021, 9, 14678-14689.</t>
+[2] M. Ramdin, A. R. T. Morrison, M. de Groen, R. van Haperen, R. de Kler, L. J. P. van den Broeke, J. P. M. Trusler, W. de Jong and T. J. H. Vlugt, Ind Eng Chem Res, 2019, 58, 1834-1847.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AH2" authorId="0" shapeId="0" xr:uid="{CE68BB1E-799F-4775-B8CB-797AF6A59114}">
+    <comment ref="AJ2" authorId="0" shapeId="0" xr:uid="{CA9200E2-D037-4AA9-A995-8A3543F0E07D}">
       <text>
         <r>
           <rPr>
@@ -638,7 +864,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -647,32 +873,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-[1] B. S. Crandall, T. Brix, R. S. Weber and F. Jiao, Energ Fuel, 2022, 37, 1441-1450.
-[2] M. Ramdin, A. R. T. Morrison, M. de Groen, R. van Haperen, R. de Kler, L. J. P. van den Broeke, J. P. M. Trusler, W. de Jong and T. J. H. Vlugt, Ind Eng Chem Res, 2019, 58, 1834-1847.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AJ2" authorId="0" shapeId="0" xr:uid="{77C5F196-F835-437B-A591-6FA79B666A10}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Yuan, Mengyao:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Use current alkaline hydrogen electrolyzer cost as a target for CO2 electrolyzer.
@@ -687,6 +888,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
+    <t>scenario</t>
+  </si>
+  <si>
     <t>run #</t>
   </si>
   <si>
@@ -696,6 +900,9 @@
     <t>target station capacity (kg/day)</t>
   </si>
   <si>
+    <t>station annual capacity factor</t>
+  </si>
+  <si>
     <t>target number of stations</t>
   </si>
   <si>
@@ -717,9 +924,30 @@
     <t>hydrogen prod. emission factor (kg CO2-eq/kg)</t>
   </si>
   <si>
+    <t>LOHC prod. emission factor (kg CO2-eq/kg)</t>
+  </si>
+  <si>
     <t>hydrogen purchase cost ($/kg)</t>
   </si>
   <si>
+    <t>LOHC purchase cost ($/kg)</t>
+  </si>
+  <si>
+    <t>LOHC name</t>
+  </si>
+  <si>
+    <t>LOHC molar mass (kg/kmol)</t>
+  </si>
+  <si>
+    <t>LOHC density (kg/m^3)</t>
+  </si>
+  <si>
+    <t>stoic. ratio (mol H2/mol LOHC)</t>
+  </si>
+  <si>
+    <t>LOHC production pathway</t>
+  </si>
+  <si>
     <t>hydr. reaction temperature (K)</t>
   </si>
   <si>
@@ -747,10 +975,25 @@
     <t>hydr. reactor energy (unit TBD)</t>
   </si>
   <si>
+    <t>hydr. LOHC output flowrate (kg/s)</t>
+  </si>
+  <si>
+    <t>hydr. electrolyzer cell area (m^2/cell)</t>
+  </si>
+  <si>
+    <t>hydr. electrolyzer voltage (V)</t>
+  </si>
+  <si>
+    <t>hydr. electrolyzer current density (A/m^2)</t>
+  </si>
+  <si>
+    <t>hydr. separator energy (unit TBD)</t>
+  </si>
+  <si>
     <t>CO2 electrolyzer purchase cost ($/m^2)</t>
   </si>
   <si>
-    <t>hydr. separator energy (unit TBD)</t>
+    <t>terminal LOHC storage amount (days)</t>
   </si>
   <si>
     <t>dehydr. reaction temperature (K)</t>
@@ -783,73 +1026,31 @@
     <t>dehydr. gas/liquid separator energy (unit TBD)</t>
   </si>
   <si>
+    <t>station LOHC storage amount (days)</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>formic acid</t>
+  </si>
+  <si>
     <t>electro</t>
   </si>
   <si>
-    <t>scenario</t>
-  </si>
-  <si>
-    <t>baseline</t>
+    <t>FA - delivery only</t>
   </si>
   <si>
     <t>purchase</t>
   </si>
   <si>
-    <t>station annual capacity factor</t>
-  </si>
-  <si>
-    <t>FA - delivery only</t>
-  </si>
-  <si>
     <t>FA - closed loop</t>
   </si>
   <si>
     <t>FA - closed loop - 80 cap factor</t>
   </si>
   <si>
-    <t>hydr. electrolyzer voltage (V)</t>
-  </si>
-  <si>
-    <t>hydr. electrolyzer current density (A/m^2)</t>
-  </si>
-  <si>
-    <t>LOHC prod. emission factor (kg CO2-eq/kg)</t>
-  </si>
-  <si>
-    <t>LOHC purchase cost ($/kg)</t>
-  </si>
-  <si>
-    <t>LOHC production pathway</t>
-  </si>
-  <si>
-    <t>terminal LOHC storage amount (days)</t>
-  </si>
-  <si>
-    <t>station LOHC storage amount (days)</t>
-  </si>
-  <si>
-    <t>LOHC name</t>
-  </si>
-  <si>
-    <t>formic acid</t>
-  </si>
-  <si>
-    <t>LOHC molar mass (kg/kmol)</t>
-  </si>
-  <si>
-    <t>LOHC density (kg/m^3)</t>
-  </si>
-  <si>
-    <t>stoic. ratio (mol H2/mol LOHC)</t>
-  </si>
-  <si>
     <t>stoic. ratio (mol CO2/mol LOHC)</t>
-  </si>
-  <si>
-    <t>hydr. LOHC output flowrate (kg/s)</t>
-  </si>
-  <si>
-    <t>hydr. electrolyzer cell area (m^2/cell)</t>
   </si>
   <si>
     <t>terminal compressed hydrogen storage amount (days)</t>
@@ -862,7 +1063,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1012,6 +1213,32 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1377,8 +1604,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1747,11 +1974,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AI3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="X3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AM1" sqref="AM1"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1765,29 +1992,29 @@
     <col min="7" max="7" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="31.85546875" customWidth="1"/>
-    <col min="32" max="32" width="34.140625" customWidth="1"/>
+    <col min="31" max="31" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="31" bestFit="1" customWidth="1"/>
@@ -1809,160 +2036,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="AJ1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="AO1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AT1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="AU1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="U1" s="2" t="s">
+      <c r="AV1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AW1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AL1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AX1" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -2023,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="V2" s="1">
         <v>366.15</v>
@@ -2053,12 +2280,12 @@
         <v>0</v>
       </c>
       <c r="AE2" s="1">
-        <f t="shared" ref="AE2:AE5" si="1">D2/2.016/S2*Q2/AP2/24/3600*F2</f>
+        <f t="shared" ref="AE2:AE5" si="1">D2*F2/2.016/S2*Q2/AP2/24/3600</f>
         <v>2.6426092969379242</v>
       </c>
       <c r="AF2" s="1">
-        <f t="shared" ref="AF2:AF5" si="2">2*96485/AH2*AE2</f>
-        <v>254.97215801505561</v>
+        <f t="shared" ref="AF2:AF5" si="2">2*96485/AH2*AE2/Q2*1000</f>
+        <v>5539.8622056503118</v>
       </c>
       <c r="AG2" s="1">
         <v>1.27</v>
@@ -2117,10 +2344,10 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B5" si="3">B2+1</f>
+        <f t="shared" ref="B3:B4" si="3">B2+1</f>
         <v>1</v>
       </c>
       <c r="C3">
@@ -2179,7 +2406,7 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="V3">
         <v>366.15</v>
@@ -2214,7 +2441,7 @@
       </c>
       <c r="AF3">
         <f t="shared" si="2"/>
-        <v>254.97215801505561</v>
+        <v>5539.8622056503118</v>
       </c>
       <c r="AG3">
         <v>1.27</v>
@@ -2273,7 +2500,7 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B4">
         <f t="shared" si="3"/>
@@ -2335,7 +2562,7 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="V4">
         <v>366.15</v>
@@ -2370,7 +2597,7 @@
       </c>
       <c r="AF4">
         <f t="shared" si="2"/>
-        <v>254.97215801505561</v>
+        <v>5539.8622056503118</v>
       </c>
       <c r="AG4">
         <v>1.27</v>
@@ -2429,10 +2656,10 @@
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B5">
-        <f t="shared" si="3"/>
+        <f>B4+1</f>
         <v>3</v>
       </c>
       <c r="C5">
@@ -2491,7 +2718,7 @@
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="V5">
         <v>366.15</v>
@@ -2526,7 +2753,7 @@
       </c>
       <c r="AF5">
         <f t="shared" si="2"/>
-        <v>254.97215801505561</v>
+        <v>5539.8622056503118</v>
       </c>
       <c r="AG5">
         <v>1.27</v>
@@ -2585,7 +2812,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:AX5">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>C3&lt;&gt;C$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2595,6 +2822,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="72d00a49-d4df-4ae2-8448-0e7c38748169">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="cdbd341c-9425-4527-8200-dbc5093c0c26" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010001B4E99C690CD84D8C14FB9B89CF5CA2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d6ebaee038f40569f500d908425f89c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="72d00a49-d4df-4ae2-8448-0e7c38748169" xmlns:ns3="cdbd341c-9425-4527-8200-dbc5093c0c26" xmlns:ns4="cc3aaed6-9815-470c-8f7f-f66d9ca72b53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0d22da384523c48d606acb8860bdc860" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="72d00a49-d4df-4ae2-8448-0e7c38748169"/>
@@ -2828,17 +3066,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="72d00a49-d4df-4ae2-8448-0e7c38748169">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="cdbd341c-9425-4527-8200-dbc5093c0c26" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2849,6 +3076,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA3A8468-9818-4804-84E1-135F70628E6B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="cc3aaed6-9815-470c-8f7f-f66d9ca72b53"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cdbd341c-9425-4527-8200-dbc5093c0c26"/>
+    <ds:schemaRef ds:uri="72d00a49-d4df-4ae2-8448-0e7c38748169"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2DAFF9-D831-4A8A-A26B-34A3990B404D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2868,17 +3113,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA3A8468-9818-4804-84E1-135F70628E6B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="72d00a49-d4df-4ae2-8448-0e7c38748169"/>
-    <ds:schemaRef ds:uri="cdbd341c-9425-4527-8200-dbc5093c0c26"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB52D826-44CA-4104-AA1D-CE7759CCAD0E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update naming for "CO2 electrolyzer"
Update parameter name to "hydr. electrolyzer" or "electrolyzer" in input file and "s2a_systems_functions.py" (code update impacts output files).
</commit_message>
<xml_diff>
--- a/systems2atoms/systems/inputs/input_params_baseline.xlsx
+++ b/systems2atoms/systems/inputs/input_params_baseline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/GitHub/systems2atoms/systems2atoms/systems/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="706" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDA50D74-30F0-4FAB-9A30-D15EFF0A634E}"/>
+  <xr:revisionPtr revIDLastSave="708" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{107B2A4B-3570-42E5-9113-5F427F326B2A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{30D85B9E-15E4-4604-8CAA-32B765517170}">
+    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{30D85B9E-15E4-4604-8CAA-32B765517170}">
       <text>
         <r>
           <rPr>
@@ -856,7 +856,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ2" authorId="0" shapeId="0" xr:uid="{CA9200E2-D037-4AA9-A995-8A3543F0E07D}">
+    <comment ref="AI2" authorId="0" shapeId="0" xr:uid="{CA9200E2-D037-4AA9-A995-8A3543F0E07D}">
       <text>
         <r>
           <rPr>
@@ -990,9 +990,6 @@
     <t>hydr. separator energy (unit TBD)</t>
   </si>
   <si>
-    <t>CO2 electrolyzer purchase cost ($/m^2)</t>
-  </si>
-  <si>
     <t>terminal LOHC storage amount (days)</t>
   </si>
   <si>
@@ -1057,6 +1054,9 @@
   </si>
   <si>
     <t>terminal liquid hydrogen storage amount (days)</t>
+  </si>
+  <si>
+    <t>hydr. electrolyzer purchase cost ($/m^2)</t>
   </si>
 </sst>
 </file>
@@ -1975,10 +1975,10 @@
   <dimension ref="A1:AX5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="X3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AH3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="AI1" sqref="AI1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2017,8 +2017,8 @@
     <col min="32" max="32" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="31" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="31" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="50" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="44.28515625" bestFit="1" customWidth="1"/>
@@ -2094,7 +2094,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>19</v>
@@ -2139,57 +2139,57 @@
         <v>32</v>
       </c>
       <c r="AI1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="AX1" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q2" s="1">
         <v>46.024999999999999</v>
@@ -2250,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V2" s="1">
         <v>366.15</v>
@@ -2280,11 +2280,11 @@
         <v>0</v>
       </c>
       <c r="AE2" s="1">
-        <f t="shared" ref="AE2:AE5" si="1">D2*F2/2.016/S2*Q2/AP2/24/3600</f>
+        <f>D2*F2/2.016/S2*Q2/AP2/24/3600</f>
         <v>2.6426092969379242</v>
       </c>
       <c r="AF2" s="1">
-        <f t="shared" ref="AF2:AF5" si="2">2*96485/AH2*AE2/Q2*1000</f>
+        <f t="shared" ref="AF2:AF5" si="1">2*96485/AH2*AE2/Q2*1000</f>
         <v>5539.8622056503118</v>
       </c>
       <c r="AG2" s="1">
@@ -2294,10 +2294,10 @@
         <v>2000</v>
       </c>
       <c r="AI2" s="1">
-        <v>0</v>
+        <v>5250</v>
       </c>
       <c r="AJ2" s="1">
-        <v>5250</v>
+        <v>0</v>
       </c>
       <c r="AK2" s="1">
         <v>0.25</v>
@@ -2344,10 +2344,10 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B4" si="3">B2+1</f>
+        <f t="shared" ref="B3:B4" si="2">B2+1</f>
         <v>1</v>
       </c>
       <c r="C3">
@@ -2391,7 +2391,7 @@
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q3">
         <v>46.024999999999999</v>
@@ -2406,7 +2406,7 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V3">
         <v>366.15</v>
@@ -2436,11 +2436,11 @@
         <v>0</v>
       </c>
       <c r="AE3">
+        <f>D3*F3/2.016/S3*Q3/AP3/24/3600</f>
+        <v>2.6426092969379242</v>
+      </c>
+      <c r="AF3">
         <f t="shared" si="1"/>
-        <v>2.6426092969379242</v>
-      </c>
-      <c r="AF3">
-        <f t="shared" si="2"/>
         <v>5539.8622056503118</v>
       </c>
       <c r="AG3">
@@ -2450,10 +2450,10 @@
         <v>2000</v>
       </c>
       <c r="AI3">
-        <v>0</v>
+        <v>5250</v>
       </c>
       <c r="AJ3">
-        <v>5250</v>
+        <v>0</v>
       </c>
       <c r="AK3">
         <v>0.25</v>
@@ -2500,10 +2500,10 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C4">
@@ -2547,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q4">
         <v>46.024999999999999</v>
@@ -2562,7 +2562,7 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V4">
         <v>366.15</v>
@@ -2592,11 +2592,11 @@
         <v>0</v>
       </c>
       <c r="AE4">
+        <f>D4*F4/2.016/S4*Q4/AP4/24/3600</f>
+        <v>2.6426092969379242</v>
+      </c>
+      <c r="AF4">
         <f t="shared" si="1"/>
-        <v>2.6426092969379242</v>
-      </c>
-      <c r="AF4">
-        <f t="shared" si="2"/>
         <v>5539.8622056503118</v>
       </c>
       <c r="AG4">
@@ -2606,10 +2606,10 @@
         <v>2000</v>
       </c>
       <c r="AI4">
-        <v>0</v>
+        <v>5250</v>
       </c>
       <c r="AJ4">
-        <v>5250</v>
+        <v>0</v>
       </c>
       <c r="AK4">
         <v>0.25</v>
@@ -2656,7 +2656,7 @@
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <f>B4+1</f>
@@ -2703,7 +2703,7 @@
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q5">
         <v>46.024999999999999</v>
@@ -2718,7 +2718,7 @@
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V5">
         <v>366.15</v>
@@ -2748,11 +2748,11 @@
         <v>0</v>
       </c>
       <c r="AE5">
+        <f>D5*F5/2.016/S5*Q5/AP5/24/3600</f>
+        <v>2.6426092969379242</v>
+      </c>
+      <c r="AF5">
         <f t="shared" si="1"/>
-        <v>2.6426092969379242</v>
-      </c>
-      <c r="AF5">
-        <f t="shared" si="2"/>
         <v>5539.8622056503118</v>
       </c>
       <c r="AG5">
@@ -2762,10 +2762,10 @@
         <v>2000</v>
       </c>
       <c r="AI5">
-        <v>0</v>
+        <v>5250</v>
       </c>
       <c r="AJ5">
-        <v>5250</v>
+        <v>0</v>
       </c>
       <c r="AK5">
         <v>0.25</v>
@@ -2833,6 +2833,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010001B4E99C690CD84D8C14FB9B89CF5CA2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d6ebaee038f40569f500d908425f89c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="72d00a49-d4df-4ae2-8448-0e7c38748169" xmlns:ns3="cdbd341c-9425-4527-8200-dbc5093c0c26" xmlns:ns4="cc3aaed6-9815-470c-8f7f-f66d9ca72b53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0d22da384523c48d606acb8860bdc860" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="72d00a49-d4df-4ae2-8448-0e7c38748169"/>
@@ -3066,15 +3075,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA3A8468-9818-4804-84E1-135F70628E6B}">
   <ds:schemaRefs>
@@ -3094,6 +3094,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB52D826-44CA-4104-AA1D-CE7759CCAD0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2DAFF9-D831-4A8A-A26B-34A3990B404D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3111,12 +3119,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB52D826-44CA-4104-AA1D-CE7759CCAD0E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Break out electrolyzer purchase cost
Break out electrolyzer purchase cost into catalyst (catalyst-coated membrane) and non-catalyst components. Add "hydr. electrolyzer catalyst cost fraction" as argument to "calcs" function (also in input .xlsx file). Link "hydr. catalyst lifetime (yr)" to electrolyzer catalyst component lifetime.
</commit_message>
<xml_diff>
--- a/systems2atoms/systems/inputs/input_params_baseline.xlsx
+++ b/systems2atoms/systems/inputs/input_params_baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/GitHub/systems2atoms/systems2atoms/systems/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="708" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{107B2A4B-3570-42E5-9113-5F427F326B2A}"/>
+  <xr:revisionPtr revIDLastSave="723" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D586893-9054-41AC-9051-F9F59DA1D1A4}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -488,8 +488,9 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Placeholder.
-Used for "thermo" formic acid production calculations, which are currently incomplete.</t>
+Use for "thermo" and "electro" LOHC production calculations. 
+Catalyst for "electro" LOHC production represents catalyst-coated membrane in electrolyzer.
+Note: "thermo" hydrogenation calculations are currently incomplete, in which case this input is a placeholder.</t>
         </r>
       </text>
     </comment>
@@ -517,7 +518,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{30D85B9E-15E4-4604-8CAA-32B765517170}">
+    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{B0EC3E37-ACB0-48CC-97D4-8D415FB5805A}">
       <text>
         <r>
           <rPr>
@@ -525,7 +526,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Yuan, Mengyao:</t>
         </r>
@@ -534,14 +535,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Currently not used.</t>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction of electrolyzer purchase cost that is attributed to catalyst components. Default value based catalyst-coated membrane cost fractions in Figure 14 in NREL, 2019, "Manufacturing Cost Analysis for Proton Exchange Membrane Water Electrolyzers", NREL/TP-6A20-72740.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AV1" authorId="0" shapeId="0" xr:uid="{3CEB65E5-8338-4451-AB5C-EBCA3C4962CC}">
+    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{30D85B9E-15E4-4604-8CAA-32B765517170}">
       <text>
         <r>
           <rPr>
@@ -565,7 +566,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{405935AC-9727-4D69-942C-356191EE2051}">
+    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{3CEB65E5-8338-4451-AB5C-EBCA3C4962CC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yuan, Mengyao:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Currently not used.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{405935AC-9727-4D69-942C-356191EE2051}">
       <text>
         <r>
           <rPr>
@@ -886,7 +911,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>scenario</t>
   </si>
@@ -1057,6 +1082,9 @@
   </si>
   <si>
     <t>hydr. electrolyzer purchase cost ($/m^2)</t>
+  </si>
+  <si>
+    <t>hydr. electrolyzer catalyst cost fraction</t>
   </si>
 </sst>
 </file>
@@ -1972,13 +2000,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX5"/>
+  <dimension ref="A1:AY5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AH3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AJ3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AI1" sqref="AI1"/>
+      <selection pane="bottomRight" activeCell="AJ1" sqref="AJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2018,24 +2046,25 @@
     <col min="33" max="33" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="31" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="50" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="31" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="29" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="43" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="31" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="50" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="31" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="29" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="43" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2142,52 +2171,55 @@
         <v>56</v>
       </c>
       <c r="AJ1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -2280,7 +2312,7 @@
         <v>0</v>
       </c>
       <c r="AE2" s="1">
-        <f>D2*F2/2.016/S2*Q2/AP2/24/3600</f>
+        <f>D2*F2/2.016/S2*Q2/AQ2/24/3600</f>
         <v>2.6426092969379242</v>
       </c>
       <c r="AF2" s="1">
@@ -2297,52 +2329,55 @@
         <v>5250</v>
       </c>
       <c r="AJ2" s="1">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="AK2" s="1">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AL2" s="1">
         <v>0.25</v>
       </c>
       <c r="AM2" s="1">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="AN2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO2" s="1">
         <v>300</v>
       </c>
-      <c r="AO2" s="1">
-        <v>1</v>
-      </c>
       <c r="AP2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="1">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AQ2" s="1">
+      <c r="AR2" s="1">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AR2" s="1">
-        <v>1</v>
-      </c>
       <c r="AS2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="1">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AT2" s="1">
+      <c r="AU2" s="1">
         <v>3500</v>
       </c>
-      <c r="AU2" s="1">
-        <v>1</v>
-      </c>
       <c r="AV2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW2" s="1">
         <v>0</v>
       </c>
       <c r="AX2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -2436,7 +2471,7 @@
         <v>0</v>
       </c>
       <c r="AE3">
-        <f>D3*F3/2.016/S3*Q3/AP3/24/3600</f>
+        <f>D3*F3/2.016/S3*Q3/AQ3/24/3600</f>
         <v>2.6426092969379242</v>
       </c>
       <c r="AF3">
@@ -2453,52 +2488,55 @@
         <v>5250</v>
       </c>
       <c r="AJ3">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="AK3">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AL3">
         <v>0.25</v>
       </c>
       <c r="AM3">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="AN3">
+        <v>1</v>
+      </c>
+      <c r="AO3">
         <v>300</v>
       </c>
-      <c r="AO3">
-        <v>1</v>
-      </c>
       <c r="AP3">
+        <v>1</v>
+      </c>
+      <c r="AQ3">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AQ3">
+      <c r="AR3">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AR3">
-        <v>1</v>
-      </c>
       <c r="AS3">
+        <v>1</v>
+      </c>
+      <c r="AT3">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AT3">
+      <c r="AU3">
         <v>3500</v>
       </c>
-      <c r="AU3">
-        <v>1</v>
-      </c>
       <c r="AV3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW3">
         <v>0</v>
       </c>
       <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -2592,7 +2630,7 @@
         <v>0</v>
       </c>
       <c r="AE4">
-        <f>D4*F4/2.016/S4*Q4/AP4/24/3600</f>
+        <f>D4*F4/2.016/S4*Q4/AQ4/24/3600</f>
         <v>2.6426092969379242</v>
       </c>
       <c r="AF4">
@@ -2609,52 +2647,55 @@
         <v>5250</v>
       </c>
       <c r="AJ4">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="AK4">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AL4">
         <v>0.25</v>
       </c>
       <c r="AM4">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="AN4">
+        <v>1</v>
+      </c>
+      <c r="AO4">
         <v>300</v>
       </c>
-      <c r="AO4">
-        <v>1</v>
-      </c>
       <c r="AP4">
+        <v>1</v>
+      </c>
+      <c r="AQ4">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AR4">
-        <v>1</v>
-      </c>
       <c r="AS4">
+        <v>1</v>
+      </c>
+      <c r="AT4">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AT4">
+      <c r="AU4">
         <v>3500</v>
       </c>
-      <c r="AU4">
-        <v>1</v>
-      </c>
       <c r="AV4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW4">
         <v>0</v>
       </c>
       <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2748,7 +2789,7 @@
         <v>0</v>
       </c>
       <c r="AE5">
-        <f>D5*F5/2.016/S5*Q5/AP5/24/3600</f>
+        <f>D5*F5/2.016/S5*Q5/AQ5/24/3600</f>
         <v>2.6426092969379242</v>
       </c>
       <c r="AF5">
@@ -2765,53 +2806,56 @@
         <v>5250</v>
       </c>
       <c r="AJ5">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="AK5">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AL5">
         <v>0.25</v>
       </c>
       <c r="AM5">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="AN5">
+        <v>1</v>
+      </c>
+      <c r="AO5">
         <v>300</v>
       </c>
-      <c r="AO5">
-        <v>1</v>
-      </c>
       <c r="AP5">
+        <v>1</v>
+      </c>
+      <c r="AQ5">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AR5">
-        <v>1</v>
-      </c>
       <c r="AS5">
+        <v>1</v>
+      </c>
+      <c r="AT5">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AT5">
+      <c r="AU5">
         <v>3500</v>
       </c>
-      <c r="AU5">
-        <v>1</v>
-      </c>
       <c r="AV5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW5">
         <v>0</v>
       </c>
       <c r="AX5">
+        <v>0</v>
+      </c>
+      <c r="AY5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:AX5">
+  <conditionalFormatting sqref="C3:AY5">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>C3&lt;&gt;C$2</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add option to use literature for dehydrogenation costs
Add input parameter for specifying reaction pathway (thermochemical, using modeled or literature results for cost calculations). Update reactor (plant) and energy costs and emissions depending on specified pathway. Rename variables for consistency.
</commit_message>
<xml_diff>
--- a/systems2atoms/systems/inputs/input_params_baseline.xlsx
+++ b/systems2atoms/systems/inputs/input_params_baseline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/GitHub/systems2atoms/systems2atoms/systems/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="774" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3F3C2BE-1301-420F-A887-1AAE14C2F64B}"/>
+  <xr:revisionPtr revIDLastSave="808" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DE93F77-7E03-4E4E-B22B-D20AC37DB302}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -565,7 +565,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX1" authorId="0" shapeId="0" xr:uid="{3CEB65E5-8338-4451-AB5C-EBCA3C4962CC}">
+    <comment ref="AY1" authorId="0" shapeId="0" xr:uid="{3CEB65E5-8338-4451-AB5C-EBCA3C4962CC}">
       <text>
         <r>
           <rPr>
@@ -585,11 +585,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Currently not used.</t>
+Unit: kWh/kg H2. 
+If dehydr. reaction pathway is "literature", use this input to account for any energy (electricity) requirements for the dehydrogenation reaction, including upstream unit operations.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AY1" authorId="0" shapeId="0" xr:uid="{405935AC-9727-4D69-942C-356191EE2051}">
+    <comment ref="AZ1" authorId="0" shapeId="0" xr:uid="{405935AC-9727-4D69-942C-356191EE2051}">
       <text>
         <r>
           <rPr>
@@ -953,7 +954,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW2" authorId="0" shapeId="0" xr:uid="{5ACBA5E6-D4BD-4257-B0A5-2524EE41A3DD}">
+    <comment ref="AX2" authorId="0" shapeId="0" xr:uid="{5ACBA5E6-D4BD-4257-B0A5-2524EE41A3DD}">
       <text>
         <r>
           <rPr>
@@ -982,7 +983,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>scenario</t>
   </si>
@@ -1041,9 +1042,6 @@
     <t>stoic. ratio (mol H2/mol LOHC)</t>
   </si>
   <si>
-    <t>LOHC production pathway</t>
-  </si>
-  <si>
     <t>hydr. reaction temperature (K)</t>
   </si>
   <si>
@@ -1113,9 +1111,6 @@
     <t>dehydr. catalyst lifetime (yr)</t>
   </si>
   <si>
-    <t>dehydr. reactor energy (unit TBD)</t>
-  </si>
-  <si>
     <t>dehydr. gas/liquid separator energy (unit TBD)</t>
   </si>
   <si>
@@ -1159,6 +1154,18 @@
   </si>
   <si>
     <t>hydr. electrolyzer lifetime (yr)</t>
+  </si>
+  <si>
+    <t>hydr. reaction pathway</t>
+  </si>
+  <si>
+    <t>dehydr. reaction pathway</t>
+  </si>
+  <si>
+    <t>thermo, model</t>
+  </si>
+  <si>
+    <t>dehydr. plant energy (kWh/kg)</t>
   </si>
 </sst>
 </file>
@@ -1753,7 +1760,17 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2074,13 +2091,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AZ5"/>
+  <dimension ref="A1:BA5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AT3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AW2" sqref="AW2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2126,20 +2143,21 @@
     <col min="39" max="39" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="50" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="31" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="29" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="43" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="24" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="31" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="29" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="43" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2198,108 +2216,111 @@
         <v>18</v>
       </c>
       <c r="T1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AL1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AZ1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AY1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="AZ1" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -2345,7 +2366,7 @@
         <v>0</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q2" s="1">
         <v>46.024999999999999</v>
@@ -2360,7 +2381,7 @@
         <v>1</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V2" s="1">
         <v>366.15</v>
@@ -2390,7 +2411,7 @@
         <v>0</v>
       </c>
       <c r="AE2" s="1">
-        <f>D2*F2/2.016/S2*Q2/AR2/24/3600</f>
+        <f>D2*F2/2.016/S2*Q2/AS2/24/3600</f>
         <v>2.6426092969379242</v>
       </c>
       <c r="AF2" s="1">
@@ -2424,43 +2445,46 @@
       <c r="AO2" s="1">
         <v>1</v>
       </c>
-      <c r="AP2" s="1">
+      <c r="AP2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ2" s="1">
         <v>300</v>
       </c>
-      <c r="AQ2" s="1">
-        <v>1</v>
-      </c>
       <c r="AR2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="1">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AS2" s="1">
+      <c r="AT2" s="1">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AT2" s="1">
-        <v>1</v>
-      </c>
       <c r="AU2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="1">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AV2" s="1">
+      <c r="AW2" s="1">
         <v>3500</v>
       </c>
-      <c r="AW2" s="1">
+      <c r="AX2" s="1">
         <v>6</v>
       </c>
-      <c r="AX2" s="1">
-        <v>0</v>
-      </c>
       <c r="AY2" s="1">
         <v>0</v>
       </c>
       <c r="AZ2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B4" si="2">B2+1</f>
@@ -2507,7 +2531,7 @@
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q3">
         <v>46.024999999999999</v>
@@ -2522,7 +2546,7 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V3">
         <v>366.15</v>
@@ -2552,7 +2576,7 @@
         <v>0</v>
       </c>
       <c r="AE3">
-        <f>D3*F3/2.016/S3*Q3/AR3/24/3600</f>
+        <f>D3*F3/2.016/S3*Q3/AS3/24/3600</f>
         <v>2.6426092969379242</v>
       </c>
       <c r="AF3">
@@ -2586,43 +2610,46 @@
       <c r="AO3">
         <v>1</v>
       </c>
-      <c r="AP3">
+      <c r="AP3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ3">
         <v>300</v>
       </c>
-      <c r="AQ3">
-        <v>1</v>
-      </c>
       <c r="AR3">
+        <v>1</v>
+      </c>
+      <c r="AS3">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AS3">
+      <c r="AT3">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AT3">
-        <v>1</v>
-      </c>
       <c r="AU3">
+        <v>1</v>
+      </c>
+      <c r="AV3">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AV3">
+      <c r="AW3">
         <v>3500</v>
       </c>
-      <c r="AW3">
+      <c r="AX3">
         <v>6</v>
       </c>
-      <c r="AX3">
-        <v>0</v>
-      </c>
       <c r="AY3">
         <v>0</v>
       </c>
       <c r="AZ3">
+        <v>0</v>
+      </c>
+      <c r="BA3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4">
         <f t="shared" si="2"/>
@@ -2669,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q4">
         <v>46.024999999999999</v>
@@ -2684,7 +2711,7 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V4">
         <v>366.15</v>
@@ -2714,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="AE4">
-        <f>D4*F4/2.016/S4*Q4/AR4/24/3600</f>
+        <f>D4*F4/2.016/S4*Q4/AS4/24/3600</f>
         <v>2.6426092969379242</v>
       </c>
       <c r="AF4">
@@ -2748,43 +2775,46 @@
       <c r="AO4">
         <v>1</v>
       </c>
-      <c r="AP4">
+      <c r="AP4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ4">
         <v>300</v>
       </c>
-      <c r="AQ4">
-        <v>1</v>
-      </c>
       <c r="AR4">
+        <v>1</v>
+      </c>
+      <c r="AS4">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AS4">
+      <c r="AT4">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AT4">
-        <v>1</v>
-      </c>
       <c r="AU4">
+        <v>1</v>
+      </c>
+      <c r="AV4">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AV4">
+      <c r="AW4">
         <v>3500</v>
       </c>
-      <c r="AW4">
+      <c r="AX4">
         <v>6</v>
       </c>
-      <c r="AX4">
-        <v>0</v>
-      </c>
       <c r="AY4">
         <v>0</v>
       </c>
       <c r="AZ4">
+        <v>0</v>
+      </c>
+      <c r="BA4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <f>B4+1</f>
@@ -2831,7 +2861,7 @@
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q5">
         <v>46.024999999999999</v>
@@ -2846,7 +2876,7 @@
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V5">
         <v>366.15</v>
@@ -2876,7 +2906,7 @@
         <v>0</v>
       </c>
       <c r="AE5">
-        <f>D5*F5/2.016/S5*Q5/AR5/24/3600</f>
+        <f>D5*F5/2.016/S5*Q5/AS5/24/3600</f>
         <v>2.6426092969379242</v>
       </c>
       <c r="AF5">
@@ -2910,42 +2940,45 @@
       <c r="AO5">
         <v>1</v>
       </c>
-      <c r="AP5">
+      <c r="AP5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ5">
         <v>300</v>
       </c>
-      <c r="AQ5">
-        <v>1</v>
-      </c>
       <c r="AR5">
+        <v>1</v>
+      </c>
+      <c r="AS5">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AT5">
-        <v>1</v>
-      </c>
       <c r="AU5">
+        <v>1</v>
+      </c>
+      <c r="AV5">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AV5">
+      <c r="AW5">
         <v>3500</v>
       </c>
-      <c r="AW5">
+      <c r="AX5">
         <v>6</v>
       </c>
-      <c r="AX5">
-        <v>0</v>
-      </c>
       <c r="AY5">
         <v>0</v>
       </c>
       <c r="AZ5">
+        <v>0</v>
+      </c>
+      <c r="BA5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:AZ5">
+  <conditionalFormatting sqref="C3:BA5">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>C3&lt;&gt;C$2</formula>
     </cfRule>
@@ -2956,15 +2989,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010001B4E99C690CD84D8C14FB9B89CF5CA2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d6ebaee038f40569f500d908425f89c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="72d00a49-d4df-4ae2-8448-0e7c38748169" xmlns:ns3="cdbd341c-9425-4527-8200-dbc5093c0c26" xmlns:ns4="cc3aaed6-9815-470c-8f7f-f66d9ca72b53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0d22da384523c48d606acb8860bdc860" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="72d00a49-d4df-4ae2-8448-0e7c38748169"/>
@@ -3198,6 +3222,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3210,14 +3243,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB52D826-44CA-4104-AA1D-CE7759CCAD0E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2DAFF9-D831-4A8A-A26B-34A3990B404D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3233,6 +3258,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB52D826-44CA-4104-AA1D-CE7759CCAD0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>